<commit_message>
Update source and template file
</commit_message>
<xml_diff>
--- a/Autobooking/SOURCE/COLLECTION BANK_20220515.xlsx
+++ b/Autobooking/SOURCE/COLLECTION BANK_20220515.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61b59f9583074f6e/98.Others/GitHub/HuongLe/Autobooking/SOURCE/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{63B1EDC7-8AEC-4D74-ADC4-923C12D30ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="DBB"/>
-    <sheet r:id="rId2" sheetId="2" name="CTB"/>
-    <sheet r:id="rId3" sheetId="3" name="VCB"/>
-    <sheet r:id="rId4" sheetId="4" name="VTB"/>
+    <sheet name="DBB" sheetId="1" r:id="rId1"/>
+    <sheet name="CTB" sheetId="2" r:id="rId2"/>
+    <sheet name="VCB" sheetId="3" r:id="rId3"/>
+    <sheet name="VTB" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Accountcol">#REF!</definedName>
     <definedName name="Assetcol">#REF!</definedName>
-    <definedName name="BU_CODE">[1]Master!$B$3</definedName>
-    <definedName name="DB_CODE">'[2]Import Header'!$C$4</definedName>
     <definedName name="T10COL">#REF!</definedName>
     <definedName name="T1COL">#REF!</definedName>
     <definedName name="T2COL">#REF!</definedName>
@@ -28,12 +32,24 @@
     <definedName name="T8COL">#REF!</definedName>
     <definedName name="T9COL">#REF!</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
   <si>
     <t>4.VIETINBANK</t>
   </si>
@@ -56,9 +72,6 @@
     <t>Doc type</t>
   </si>
   <si>
-    <t>Doc date</t>
-  </si>
-  <si>
     <t>ACC_VTB001</t>
   </si>
   <si>
@@ -161,24 +174,6 @@
     <t>Thu tien KH nop tai VCB (unpair)-dd.mm.yy</t>
   </si>
   <si>
-    <t>Posting date</t>
-  </si>
-  <si>
-    <t>File date</t>
-  </si>
-  <si>
-    <t>Document date</t>
-  </si>
-  <si>
-    <t>LR --&gt; IFRS 101* --&gt; luôn có data --&gt; item text --&gt; document date</t>
-  </si>
-  <si>
-    <t>Item text date</t>
-  </si>
-  <si>
-    <t>Text trên file</t>
-  </si>
-  <si>
     <t>2.CITIBANK</t>
   </si>
   <si>
@@ -221,15 +216,6 @@
     <t>Thu tien KH nop tai Citi (unpair)-dd.mm.yy</t>
   </si>
   <si>
-    <t>LJ --&gt; chỉ có 1 dòng *trong ngay* --&gt; luôn có data --&gt; item text --&gt; document date</t>
-  </si>
-  <si>
-    <t>hoặc</t>
-  </si>
-  <si>
-    <t>LJ --&gt; chỉ có 1 dòng *phat sinh* --&gt; luôn có data --&gt; item text --&gt; document date</t>
-  </si>
-  <si>
     <t>1.DEUTSCHE BANK</t>
   </si>
   <si>
@@ -273,16 +259,12 @@
   </si>
   <si>
     <t>Thu tien KH nop tai DB (unpair)-dd.mm.yy</t>
-  </si>
-  <si>
-    <t>LJ --&gt; check IFRS = 101*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -306,7 +288,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -320,17 +302,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdae3f3"/>
+        <fgColor rgb="FFDAE3F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFc2a3ff"/>
+        <fgColor rgb="FFC2A3FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -359,16 +341,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -399,97 +381,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -500,10 +477,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -541,71 +518,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -633,7 +610,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -656,11 +633,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -669,13 +646,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -685,7 +662,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -694,7 +671,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -703,7 +680,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -711,10 +688,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -779,31 +756,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="21" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="21" width="43.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="22" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="22" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="21" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="21" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="21" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="21" width="21.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="22.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -825,123 +801,125 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C2" s="8">
         <f>SUM(D2:D7)-SUM(C3:C7)</f>
+        <v>0</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="11">
+        <v>59</v>
+      </c>
+      <c r="G2" s="11" t="str">
         <f>IF($C$2&gt;0,"LR","LJ")</f>
+        <v>LJ</v>
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21">
+    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="13">
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21">
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
+    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="9"/>
       <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="13"/>
       <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="13"/>
       <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="16"/>
@@ -951,7 +929,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="16"/>
@@ -961,7 +939,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="16"/>
@@ -971,11 +949,9 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21">
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="23" t="s">
-        <v>80</v>
-      </c>
+      <c r="B11" s="23"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="5"/>
@@ -989,31 +965,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="21" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="21" width="43.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="22" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="27" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="22" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="21" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="21" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="22" width="21.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="22.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1035,34 +1012,36 @@
       </c>
       <c r="H1" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C2" s="8">
         <f>SUM(D2:D7)-SUM(C3:C7)</f>
+        <v>0</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="24">
         <v>101050010</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="11">
+        <v>44</v>
+      </c>
+      <c r="G2" s="11" t="str">
         <f>IF($C$2&gt;0,"LR","LJ")</f>
+        <v>LJ</v>
       </c>
       <c r="H2" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21">
+    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="13"/>
@@ -1070,17 +1049,17 @@
         <v>901010002</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21">
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="13"/>
@@ -1088,17 +1067,17 @@
         <v>901010002</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
+    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="9"/>
@@ -1106,17 +1085,17 @@
         <v>901010002</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="13"/>
@@ -1124,17 +1103,17 @@
         <v>901010002</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="13"/>
@@ -1142,24 +1121,25 @@
         <v>2999000001</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21">
+    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17">
         <f>SUM(C2:C7)-SUM(D2:D7)</f>
+        <v>0</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="16"/>
@@ -1169,7 +1149,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="16"/>
@@ -1179,7 +1159,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="16"/>
@@ -1189,7 +1169,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="16"/>
@@ -1199,13 +1179,9 @@
       <c r="G12" s="5"/>
       <c r="H12" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21">
-      <c r="A13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>43</v>
-      </c>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="16"/>
       <c r="D13" s="26"/>
       <c r="E13" s="16"/>
@@ -1213,27 +1189,19 @@
       <c r="G13" s="5"/>
       <c r="H13" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21">
-      <c r="A14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>62</v>
-      </c>
+    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="16"/>
       <c r="D14" s="26"/>
-      <c r="E14" s="25" t="s">
-        <v>63</v>
-      </c>
+      <c r="E14" s="25"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="21">
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="23" t="s">
-        <v>64</v>
-      </c>
+      <c r="B15" s="23"/>
       <c r="C15" s="16"/>
       <c r="D15" s="26"/>
       <c r="E15" s="16"/>
@@ -1241,13 +1209,9 @@
       <c r="G15" s="5"/>
       <c r="H15" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21">
-      <c r="A16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>47</v>
-      </c>
+    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="16"/>
       <c r="D16" s="26"/>
       <c r="E16" s="16"/>
@@ -1255,7 +1219,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="16"/>
@@ -1265,7 +1229,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="16"/>
@@ -1275,59 +1239,47 @@
       <c r="G18" s="5"/>
       <c r="H18" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="21">
+    <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="16"/>
-      <c r="D19" s="17">
-        <v>187</v>
-      </c>
+      <c r="D19" s="17"/>
       <c r="E19" s="16"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="21">
+    <row r="20" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="16"/>
-      <c r="D20" s="17">
-        <v>189</v>
-      </c>
+      <c r="D20" s="17"/>
       <c r="E20" s="16"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="21">
+    <row r="21" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="17">
-        <v>284</v>
-      </c>
+      <c r="D21" s="17"/>
       <c r="E21" s="16"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="21">
+    <row r="22" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="17">
-        <f>SUM(D19:D21)</f>
-      </c>
-      <c r="E22" s="25">
-        <f>D22+1259</f>
-      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="17">
-        <f>73+35</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="16"/>
@@ -1337,13 +1289,11 @@
       <c r="G23" s="5"/>
       <c r="H23" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="21">
+    <row r="24" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="17">
-        <f>250*8</f>
-      </c>
+      <c r="D24" s="17"/>
       <c r="E24" s="16"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1355,31 +1305,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="20" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="21" width="43.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="22" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="22" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="21" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="21" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="21" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="21" width="21.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="22.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1401,135 +1350,135 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="C2" s="8">
         <f>SUM(D2:D7)-SUM(C3:C7)</f>
+        <v>225221224</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="11" t="str">
+        <f>IF($C$2&gt;0,"LR","LJ")</f>
+        <v>LR</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="11">
-        <f>IF($C$2&gt;0,"LR","LJ")</f>
-      </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="13"/>
       <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21">
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="13">
         <v>220937224</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
+    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="9"/>
       <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="13"/>
       <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="13">
         <v>4284000</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21">
+    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="5"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="17">
-        <f>SUM(C2:C7)-SUM(D2:D7)</f>
-      </c>
+      <c r="D8" s="17"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="5"/>
       <c r="C9" s="16"/>
@@ -1539,7 +1488,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="5"/>
       <c r="C10" s="16"/>
@@ -1549,13 +1498,9 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21">
-      <c r="A11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>43</v>
-      </c>
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="5"/>
@@ -1563,13 +1508,9 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21">
-      <c r="A12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>45</v>
-      </c>
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="5"/>
@@ -1577,13 +1518,9 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21">
-      <c r="A13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>47</v>
-      </c>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="5"/>
@@ -1597,30 +1534,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="20" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="21" width="43.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="22" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="22" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="21" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="21" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="21" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="21" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="21" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="22.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1642,141 +1578,140 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="8">
         <f>SUM(D2:D7)-SUM(C3:C7)</f>
+        <v>3490655339</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="11" t="str">
+        <f>IF($C$2&gt;0,"LR","LJ")</f>
+        <v>LR</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="11">
-        <f>IF($C$2&gt;0,"LR","LJ")</f>
-      </c>
-      <c r="H2" s="11">
-        <f>RIGHT(B2,8)</f>
-      </c>
-      <c r="I2" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="13"/>
       <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="14"/>
       <c r="I3" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="13">
         <v>3322684406</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="14"/>
       <c r="I4" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="9"/>
       <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="14"/>
       <c r="I5" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="13"/>
       <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="14"/>
       <c r="I6" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="13">
         <v>167970933</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="14"/>
       <c r="I7" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="5"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17">
         <f>SUM(C2:C7)-SUM(D2:D7)</f>
+        <v>0</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -1784,7 +1719,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="5"/>
       <c r="C9" s="16"/>
@@ -1795,7 +1730,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="5"/>
       <c r="C10" s="16"/>
@@ -1806,12 +1741,12 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -1821,12 +1756,12 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -1836,12 +1771,12 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>

</xml_diff>